<commit_message>
nice Excel for Data doenload
</commit_message>
<xml_diff>
--- a/Titelblatt.xlsx
+++ b/Titelblatt.xlsx
@@ -5,22 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sszfea\GitHub\Shiny-Apps\MPE-Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Ablageordner\ABDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="7245" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="7245"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Erläuterungen" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Napfgasse 6, 8022 Zürich</t>
   </si>
@@ -61,74 +60,14 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Begriff</t>
-  </si>
-  <si>
-    <t>Definition</t>
-  </si>
-  <si>
-    <t>Mietpreiserhebung (MPE)</t>
-  </si>
-  <si>
-    <t>Die Mietpreiserhebung (MPE) gibt die geschätzten Mietpreise in der Stadt Zürich per Stichmonat April 2022 wieder. Die Erhebung ist als Zweischichtenmodell konzipiert und basiert auf automatisierten Datenlieferungen von Verwaltungen (Schicht 1) und einer ergänzenden Zufallsstichprobe (Schicht 2). Die Resultate beziehen sich ausschliesslich auf die Grössenklassen der 2-, 3- und 4-Zimmer-Wohnungen, die über 80 Prozent des Mietwohnungsbestandes abdecken. Vgl. auch den publizierten Methodikbericht.</t>
-  </si>
-  <si>
-    <t>Gemeinnützigkeit</t>
-  </si>
-  <si>
-    <t>Zu den gemeinnützigen gehören zunächst alle Wohnungen, die im Besitz der Stadt oder von Genossenschaften, Vereinen oder Stiftungen sind und nach dem Grundsatz der Kostenmiete bewirtschaftet werden. Ferner gehören auch Wohnungen dazu, deren Eigentümerschaft als gemeinnützig im weiteren Sinne gilt und ihre Mietobjekte nicht ausschliesslich nach dem Prinzip der Kostenmiete vermietet (bestimmte Stiftungen, Vereine und Aktiengesellschaften). Mit der Kostenmiete werden die Schuldzinsen und die Verwaltungskosten beglichen, der Unterhalt und Werterhalt der Liegenschaften sowie die Rückstellungen zur Erneuerung sichergestellt. Mittel- bis langfristig bewirkt die Kostenmiete deutlich günstigere Mieten als bei vergleichbaren Objekten auf dem Wohnungsmarkt.</t>
-  </si>
-  <si>
-    <t>Median (Zentralwert)</t>
-  </si>
-  <si>
-    <t>Konfidenzintervall</t>
-  </si>
-  <si>
-    <t>Abfragetool MPE</t>
-  </si>
-  <si>
     <t>Platzhalter: Titel der Tabelle</t>
-  </si>
-  <si>
-    <t>Total Wohnungen (Domain)</t>
-  </si>
-  <si>
-    <t>Anzahl Wohnungen in Sample 1 bzw. Sample 2</t>
-  </si>
-  <si>
-    <t>Grundgesamtheit für die betreffende Zelle: Gesamtzahl der Wohnungen der betreffenden Kategorie (Ausprägung von Raumeinheit, Gliederung, Zimmerzahl und Art der Gemeinnützigkeit).</t>
-  </si>
-  <si>
-    <t>Filterung nach Bauträgerschaft</t>
-  </si>
-  <si>
-    <t>Da bei kleinen Stadtquartieren aufgrund von zu geringen Datenmengen keine Differenzierung der Mietpreise nach Bauträgerschaft (gemeinnützig oder nicht gemeinnützig) möglich ist, werden die Kreise 1, 2, 5 und 8 nicht in die einzelnen Quartiere aufgeteilt, sowie folgende Quartiergruppen gebildet: Fluntern und Hottingen, Hirslanden und Witikon, Alt-Wiedikon und Friesenberg, Werd und Langstrasse sowie Saatlen und Schwamendingen-Mitte.</t>
-  </si>
-  <si>
-    <t>Raumeinheit Quartiergruppe</t>
-  </si>
-  <si>
-    <t>Diese Raumeinheit wurde aufgrund der Filterung nach Bauträgerschaft gebildet. Siehe entsprechender Abschnitt.</t>
-  </si>
-  <si>
-    <t>Der Median ist der Wert, der die Mietpreise in zwei gleich grosse Hälften teilt, d.h. die eine Hälfte der Mietpreise kleiner als der Median, die andere Hälfte grösser.</t>
-  </si>
-  <si>
-    <t>Die geschätzten Preise sind mit 95-%-Konfidenzintervallen unterlegt. Diese bezeichnen den Bereich, der bei unendlicher Wiederholung eines Zufallsexperiments mit einer Wahrscheinlichkeit von 95 Prozent den wahren Wert der Grundgesamtheit einschliesst. In der MPE liegen die 95-%-Konfidenzintervalle gesamtstädtisch ungefähr bei 4 Prozent der ausgewiesenen Medianpreise und Mittelwerte (absolute Breite des Konfidenzintervalls geteilt durch Schätzwert). Bei kleineren Raumeinheiten (z.B. Quartiere) sind die Unsicherheiten höher; die Konfidenzintervalle der ausgewiesenen Werte liegen im Bereich von 4 bis 8 Prozent und können unter Umständen bis gegen 20 Prozent steigen.</t>
-  </si>
-  <si>
-    <t>Samplegrösse für die betreffende Zelle pro Schicht 1 resp. Schicht 2: Anzahl Mietpreisinformationen, die vorliegen.</t>
-  </si>
-  <si>
-    <t>Die Detaildaten der Mietpreiserhebung 2022 sind auf einem Abruftool verfügbar, das erreichbar ist unter: https://www.stadt-zuerich.ch/prd/de/index/statistik/publikationen-angebote/datenbanken-anwendungen/mietpreiserhebung.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,45 +80,8 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -204,36 +106,12 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -483,7 +361,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -547,112 +425,11 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.39370078740157483" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.27559055118110237"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="27.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" s="5" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.71" right="0.71" top="0.98" bottom="0.59" header="0.4" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>